<commit_message>
Added more detailed comments on Python libraries and version to use
</commit_message>
<xml_diff>
--- a/KeywordExtraction/Results_Detailed Accuracy/detailedAccuracy.xlsx
+++ b/KeywordExtraction/Results_Detailed Accuracy/detailedAccuracy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="258">
   <si>
     <t>Original Text</t>
   </si>
@@ -25,238 +25,769 @@
     <t>Confidence Level</t>
   </si>
   <si>
-    <t>hey guys welcome back so today</t>
-  </si>
-  <si>
-    <t>I thought is a full body workout</t>
-  </si>
-  <si>
-    <t>that's gonna work multiple muscle groups at the same time</t>
-  </si>
-  <si>
-    <t>it's also gonna help you to burn fat</t>
-  </si>
-  <si>
-    <t>this workout is part of a lean dance program and you can find the full schedule over here</t>
-  </si>
-  <si>
-    <t>now don't forget to snap some progress photos and videos so you can share it with the rest of us and also hit that thumbs up button subscribe internal caches</t>
-  </si>
-  <si>
-    <t>and let's get started</t>
-  </si>
-  <si>
-    <t>we have 24 exercises today</t>
-  </si>
-  <si>
-    <t>most exercises are 30 seconds with five seconds</t>
-  </si>
-  <si>
-    <t>rest in between</t>
-  </si>
-  <si>
-    <t>let's start with butt kickers (3 second silence) kick up your legs behind you fast load and bring up the speed for low impact you can just take it (20 second silence) slow (3 second silence) now with lunch tab lunch slightly to one side and touch your toe with your opposite hand (30 second silence) now</t>
-  </si>
-  <si>
-    <t>we have snowboarding jump squats</t>
-  </si>
-  <si>
-    <t>Luis squats and take a 90 degrees</t>
-  </si>
-  <si>
-    <t>jump to the other side</t>
-  </si>
-  <si>
-    <t>then do another squat and repeat for low impact you can just do the (21 second silence) squat (4 second silence) get ready for some high knees</t>
-  </si>
-  <si>
-    <t>bring your knee up to a hip level and get your core and do it as fast as you can</t>
-  </si>
-  <si>
-    <t>you can do it for low impact</t>
-  </si>
-  <si>
-    <t>just raise the knee up without the jump (24 second silence) now we have double hop burpees</t>
-  </si>
-  <si>
-    <t>starting high playing then jumbo feet in and out and eat again</t>
-  </si>
-  <si>
-    <t>then get up and do another jump off the ground for low impact just do burpees with other job (23 second silence)</t>
-  </si>
-  <si>
-    <t>now we have jumping jacks</t>
-  </si>
-  <si>
-    <t>let's do this as fast as you can</t>
-  </si>
-  <si>
-    <t>and make sure your coils tight work</t>
-  </si>
-  <si>
-    <t>those muscles (27 second silence)</t>
-  </si>
-  <si>
-    <t>now we have squat with oblique</t>
-  </si>
-  <si>
-    <t>crunch for one whole minute squat down and do a twister punch as you get up</t>
-  </si>
-  <si>
-    <t>this works your legs</t>
-  </si>
-  <si>
-    <t>butt and abs at the same (2 second silence) time (29 second silence) super amazing</t>
-  </si>
-  <si>
-    <t>all right now we have a 15 seconds break and you can take a longer break if you want to</t>
-  </si>
-  <si>
-    <t>we have push up toe tap next</t>
-  </si>
-  <si>
-    <t>start with push up and then touch your toe with your opposite hand</t>
-  </si>
-  <si>
-    <t>if you can't do a regular push up you can start with just toe tap only that eventually you can add some push ups or you can try</t>
-  </si>
-  <si>
-    <t>knee push ups (9 second silence) now (18 second silence) flip around and have your elbow resting on a mat</t>
-  </si>
-  <si>
-    <t>we are doing bicycles next</t>
-  </si>
-  <si>
-    <t>this works your abs</t>
-  </si>
-  <si>
-    <t>so keep pushing (27 second silence)</t>
-  </si>
-  <si>
-    <t>now we have up and down with two jacks make sure your core is engaged</t>
-  </si>
-  <si>
-    <t>come on guys you can do it</t>
-  </si>
-  <si>
-    <t>(29 second silence)</t>
-  </si>
-  <si>
-    <t>now we have be up with straight leg crunch</t>
-  </si>
-  <si>
-    <t>try your best to do this in good form and I hope your ass is on fire right now</t>
-  </si>
-  <si>
-    <t>(27 second silence) mountain climbers is next</t>
-  </si>
-  <si>
-    <t>tighten up their ass and crank up the speed guys</t>
-  </si>
-  <si>
-    <t>we're halfway through the workout</t>
-  </si>
-  <si>
-    <t>let's smash this (27 second silence) next we side plank with a kick down tabletop with the Cape start in a site playing then</t>
-  </si>
-  <si>
-    <t>kick the top light in front of you</t>
-  </si>
-  <si>
-    <t>then bring the leg back and get into a tabletop position and kick the other leg up touching your hand</t>
-  </si>
-  <si>
-    <t>if this is too hot you can do a side plank hole (18 second silence) now</t>
-  </si>
-  <si>
-    <t>let's do the same on the other side do it</t>
-  </si>
-  <si>
-    <t>slow and steady</t>
-  </si>
-  <si>
-    <t>if you need to the exercise (29 second silence) now we have walking plank</t>
-  </si>
-  <si>
-    <t>walk both legs and hands a site to site</t>
-  </si>
-  <si>
-    <t>make sure your butt is not poking up and squeeze those abs (27 second silence)</t>
-  </si>
-  <si>
-    <t>let's take a quick 15 second break</t>
-  </si>
-  <si>
-    <t>you can also take a longer break</t>
-  </si>
-  <si>
-    <t>if you want to</t>
-  </si>
-  <si>
-    <t>(7 second silence)</t>
-  </si>
-  <si>
-    <t>let's do some squats oblique crunch for another 30 seconds</t>
-  </si>
-  <si>
-    <t>squat low guys work those legs and back and also your abs (26 second silence) now squat a little and take a little hop with one leg to the side for low impact</t>
-  </si>
-  <si>
-    <t>you can just take a step without the hop (28 second silence)</t>
-  </si>
-  <si>
-    <t>we're shuffle crunch next shuffle to one side and crunch and then to the other side you can do just a crunch only for the low impact version (26 second silence) next work in</t>
-  </si>
-  <si>
-    <t>Mount jump and bring both of the legs out and then in do it fast but make sure you are doing it in good form core tight back neutral and all muscles activate it for low impact</t>
-  </si>
-  <si>
-    <t>just bring one leg out at one time and bring them back</t>
-  </si>
-  <si>
-    <t>(6 second silence) in (13 second silence)</t>
-  </si>
-  <si>
-    <t>now let's do some standing crunches</t>
-  </si>
-  <si>
-    <t>we are almost done with the workout</t>
-  </si>
-  <si>
-    <t>guys keep pushing (29 second silence) we have lateral lunge</t>
-  </si>
-  <si>
-    <t>we've jumped next</t>
-  </si>
-  <si>
-    <t>bring one leg to the side and lash down then climb back up to the center and jump up below impact just two letter lunch only without the jump (24 second silence)</t>
-  </si>
-  <si>
-    <t>let's do the same on the other side</t>
-  </si>
-  <si>
-    <t>(33 second silence) we're plank will show the tap next do it fast and keep your core engaged</t>
-  </si>
-  <si>
-    <t>try not to sway too much and we have one more exercise to go</t>
-  </si>
-  <si>
-    <t>let's finish this workout (24 second silence) the final exercises</t>
-  </si>
-  <si>
-    <t>Heine bring up your knee up to hips level</t>
-  </si>
-  <si>
-    <t>do it as fast as you can</t>
-  </si>
-  <si>
-    <t>core tight and we'll only have a couple of more seconds to (24 second silence) go</t>
-  </si>
-  <si>
-    <t>that's the workout guys who've done well don't forget to smash that like button</t>
-  </si>
-  <si>
-    <t>subscribe internal applications so that you don't miss out on my new program and I'll see you in the next workout</t>
+    <t>hey everybody it's your personal trainer coach</t>
+  </si>
+  <si>
+    <t>&lt;unk&gt; here from has fake</t>
+  </si>
+  <si>
+    <t>and i'm claudia</t>
+  </si>
+  <si>
+    <t>and this is our beginner weight training routine</t>
+  </si>
+  <si>
+    <t>this routine is great for both men and women of a beginner fitness level</t>
+  </si>
+  <si>
+    <t>the only equipment required for this workout is a pair of dumbbells now</t>
+  </si>
+  <si>
+    <t>that weight of the dumbbells is going to be totally determined by your current fitness level</t>
+  </si>
+  <si>
+    <t>just remember it's much better to start light and work your way up than the other way around the only only other equipment that you may want for</t>
+  </si>
+  <si>
+    <t>this workout is a chair or a box for some of the modified movements</t>
+  </si>
+  <si>
+    <t>we're going to do the whole thing with you</t>
+  </si>
+  <si>
+    <t>ready to get this thing going all right we're going to start with either a dumbbell &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>or a dumbbell &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>so if you want to do the easier modified versions you go and follow claudia</t>
+  </si>
+  <si>
+    <t>she's going to be using one dumbbell</t>
+  </si>
+  <si>
+    <t>i'm going to use two</t>
+  </si>
+  <si>
+    <t>so that's the main difference</t>
+  </si>
+  <si>
+    <t>i'm going to squeeze these together and i'm going to pull back and claudia is just going to &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>her fingers and pull back either way</t>
+  </si>
+  <si>
+    <t>we're both pulling back on our elbows</t>
+  </si>
+  <si>
+    <t>keeping those elbows tucked in nice and tight to the body pulling back we're keeping our core tight and straight and our upper body is on a &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>degree angle</t>
+  </si>
+  <si>
+    <t>now we're not going to count any repetitions today</t>
+  </si>
+  <si>
+    <t>i just want you to try to perform as many moves as you can in allotted time period work at your own pace but at the same time be sure to push yourself because nobody else can do it for you</t>
+  </si>
+  <si>
+    <t>three nice work keep it going pulling back on those elbows keeping them tight to your body in five four three two and one okay</t>
+  </si>
+  <si>
+    <t>we're going to go to the ground for the next one</t>
+  </si>
+  <si>
+    <t>it's going to be a combo movement</t>
+  </si>
+  <si>
+    <t>we're going to need both weights for this one</t>
+  </si>
+  <si>
+    <t>we're going to do a hip up plus chest press</t>
+  </si>
+  <si>
+    <t>we're going to drive off our heels and at the same time we're going to press the dumbbell straight up and back down getting a lot of different body parts worked in this one</t>
+  </si>
+  <si>
+    <t>so we're getting your hamstrings your &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>your lower back your abs just shoulders triceps</t>
+  </si>
+  <si>
+    <t>the list goes on but it's a very efficient movement getting a lot of work in in a short period of time drive off those heels</t>
+  </si>
+  <si>
+    <t>squeeze the gluts up at the top</t>
+  </si>
+  <si>
+    <t>try your best not to &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>your back to just come up until your upper body is in this nice straight line and make sure not to bounce your arms off the ground either nice work breathe one right into the next moving at a pace that you feel comfortable with you got it almost there</t>
+  </si>
+  <si>
+    <t>let's go five more seconds on this one and four three two one and done okay</t>
+  </si>
+  <si>
+    <t>we're on to our feet for the next one need both weights again</t>
+  </si>
+  <si>
+    <t>we're going to either do a stiff leg &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>plus shrug or claudia is going to show you an ar</t>
+  </si>
+  <si>
+    <t>deal with chance for romanian &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>i didn't make that up shrug either way</t>
+  </si>
+  <si>
+    <t>we're going to put our weight back in our hips</t>
+  </si>
+  <si>
+    <t>little bend the knee</t>
+  </si>
+  <si>
+    <t>i'm going to go all the way down</t>
+  </si>
+  <si>
+    <t>and i'm going to bring my hips forward and shrug claudia's just going to come</t>
+  </si>
+  <si>
+    <t>and bring her hands just below our knees and then repeat that same shrug</t>
+  </si>
+  <si>
+    <t>so we're driving our hips backwards</t>
+  </si>
+  <si>
+    <t>all the way up hips forward</t>
+  </si>
+  <si>
+    <t>and then shrug bringing your shoulders up to your ears</t>
+  </si>
+  <si>
+    <t>feel that stretching your hamstrings</t>
+  </si>
+  <si>
+    <t>if you're not feeling a stretch in the back of your leg then i want to make sure you drive in those hips back just a little bit in those knees and hips</t>
+  </si>
+  <si>
+    <t>go back again</t>
+  </si>
+  <si>
+    <t>another combo movement this one feet in hamstrings &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>lower back and your traps good and notice how both of us are keeping our backs</t>
+  </si>
+  <si>
+    <t>nice and straight on this movement so we're not breaking that straight line and punching over but keeping our back straight while we're kicking those hips back you got it almost done with this one five four three two and last one zero nice okay</t>
+  </si>
+  <si>
+    <t>so we're going to move on to some shoulder presses next</t>
+  </si>
+  <si>
+    <t>i'm gonna grab my box over here</t>
+  </si>
+  <si>
+    <t>claudia's going to grab our box</t>
+  </si>
+  <si>
+    <t>and i'm going to do this</t>
+  </si>
+  <si>
+    <t>one from a standing position so from the box</t>
+  </si>
+  <si>
+    <t>it's a little easier standing a little harder standing it forces me to use a little bit more stability and a little bit more core but overall very comparable movements</t>
+  </si>
+  <si>
+    <t>you decide which one is right for you if you don't feel comfortable the overhead quite yet grab a seat full range of motion on this one all the way up all the way down</t>
+  </si>
+  <si>
+    <t>stay nice and under control you want to fling or swing the dumbbells around keep your core tight</t>
+  </si>
+  <si>
+    <t>this is a strength training routine so we don't want to</t>
+  </si>
+  <si>
+    <t>i know you said work at your own pace</t>
+  </si>
+  <si>
+    <t>but we definitely don't want to make this a cardio and just start pumping out correct exactly right if you using a weight that you can just do &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>reps in this &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>second time period</t>
+  </si>
+  <si>
+    <t>then you up the weight nice okay not much time left on this one</t>
+  </si>
+  <si>
+    <t>(2 second silence) and five four</t>
+  </si>
+  <si>
+    <t>three two and one</t>
+  </si>
+  <si>
+    <t>nice all right shake the arm</t>
+  </si>
+  <si>
+    <t>move this out of the way and we're going to move into a dumbbell curl so we're gonna hit those biceps next working on the gun show &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>got to go and show her tank top on tonight with those guns anyway</t>
+  </si>
+  <si>
+    <t>firing my wife's guns okay</t>
+  </si>
+  <si>
+    <t>so we're going to do a curl</t>
+  </si>
+  <si>
+    <t>both palms come up</t>
+  </si>
+  <si>
+    <t>we're going to curl those &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>in on the way up and then all the way back down again</t>
+  </si>
+  <si>
+    <t>this one's under control</t>
+  </si>
+  <si>
+    <t>so that means we're not swinging up and flinging them back down right it defeats the purpose but instead i feel that time under tension feel those muscles contracting all the way up and all the way down you got it good closing give you a nice side view</t>
+  </si>
+  <si>
+    <t>keep those shoulders back and square</t>
+  </si>
+  <si>
+    <t>mm &lt;unk&gt; you got it</t>
+  </si>
+  <si>
+    <t>we're breathing just &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>more seconds left on this one flight through you got it and three two one and zero are moving to the lower body</t>
+  </si>
+  <si>
+    <t>claudia is going to grab her box or if you have a chair that works as well if you want to the modified version</t>
+  </si>
+  <si>
+    <t>i'm also going to lose a dumbbell here</t>
+  </si>
+  <si>
+    <t>yeah &lt;unk&gt; exactly she's only gonna use one way good point so she's going to do a goblet squats</t>
+  </si>
+  <si>
+    <t>she notice how she's holding the way up two hands and i got a new thumbs out</t>
+  </si>
+  <si>
+    <t>i'm not gonna do a dumbbell squat just with at my side so i'm going to go up</t>
+  </si>
+  <si>
+    <t>be able to get a little bit deeper</t>
+  </si>
+  <si>
+    <t>then doing the chair or box squat</t>
+  </si>
+  <si>
+    <t>but either way we're both bending at the hips first driving those hips back and then coming down until our hips are parallel to the ground</t>
+  </si>
+  <si>
+    <t>all the way up all the way down and i'm just touching the chair and coming right back up</t>
+  </si>
+  <si>
+    <t>i'm not sitting not resting exactly</t>
+  </si>
+  <si>
+    <t>i make sure you're bouncing</t>
+  </si>
+  <si>
+    <t>that's the other thing right</t>
+  </si>
+  <si>
+    <t>correct on swing off of this</t>
+  </si>
+  <si>
+    <t>if you guys still shave you hear the seat either or squatting make sure you keep those knees out</t>
+  </si>
+  <si>
+    <t>don't allow them to break your compress in nice work</t>
+  </si>
+  <si>
+    <t>how much left on this one</t>
+  </si>
+  <si>
+    <t>i know your legs are probably starting to feel it</t>
+  </si>
+  <si>
+    <t>i didn't forget about you</t>
+  </si>
+  <si>
+    <t>we got five four three two and one done okay</t>
+  </si>
+  <si>
+    <t>we're going to move on to a dumbbell &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>kickback we're gonna hit those triceps</t>
+  </si>
+  <si>
+    <t>next save movement really just to put a mix up your weight find</t>
+  </si>
+  <si>
+    <t>what weight works for you on this one</t>
+  </si>
+  <si>
+    <t>so we're bent over our elbows are up</t>
+  </si>
+  <si>
+    <t>we're only going to bend at those elbows not moving the whole arm</t>
+  </si>
+  <si>
+    <t>keep your core tight and at the top</t>
+  </si>
+  <si>
+    <t>you're squeezing that back of the arm squeezing your triceps up at the top nice work notice</t>
+  </si>
+  <si>
+    <t>we're using that elbow as a lever</t>
+  </si>
+  <si>
+    <t>so we're not moving that upper arm</t>
+  </si>
+  <si>
+    <t>just bend at the elbow so i mean but as you're not going here right now singing no swinging because now all the sudden all the other muscles are taking over we just want to isolate the triceps on this one you got it ten more seconds</t>
+  </si>
+  <si>
+    <t>that's it guys are doing great</t>
+  </si>
+  <si>
+    <t>thank you so much for joining us today and for all of your hard work and three two one and done</t>
+  </si>
+  <si>
+    <t>okay we're going to the ground losing my weights body's going to lose your weights</t>
+  </si>
+  <si>
+    <t>i'm going to keep mine though we're going to do a dumbbell reach crunch so from a crunch position we're going to our feet on the ground</t>
+  </si>
+  <si>
+    <t>we're going to reach up to the ceiling</t>
+  </si>
+  <si>
+    <t>we're going our shoulder blades</t>
+  </si>
+  <si>
+    <t>off the ground and come back down to earth contracting the abs up at the top reaching up big and high you see i'm using my weights making it more difficult claudia</t>
+  </si>
+  <si>
+    <t>she's just using her body weight</t>
+  </si>
+  <si>
+    <t>you could also just use one way if you wanted to straight so again</t>
+  </si>
+  <si>
+    <t>it's all about making this your own coming back repeating it getting a little bit better every single time and that's how we improve that consistency</t>
+  </si>
+  <si>
+    <t>nice work reaching up</t>
+  </si>
+  <si>
+    <t>don't bounce off the ground stay under control you got it nice work nice work</t>
+  </si>
+  <si>
+    <t>we got 10 more seconds on this one beyond those abs start to work</t>
+  </si>
+  <si>
+    <t>that's a good thing</t>
+  </si>
+  <si>
+    <t>that's the feeling of improvement right there and three two one and zero okay</t>
+  </si>
+  <si>
+    <t>we're going to rest</t>
+  </si>
+  <si>
+    <t>that's the end of the first round</t>
+  </si>
+  <si>
+    <t>we got one more to go all right</t>
+  </si>
+  <si>
+    <t>so it's a quick &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>second break that doesn't give you much time</t>
+  </si>
+  <si>
+    <t>if you want</t>
+  </si>
+  <si>
+    <t>feel free to grab some water shake it loose</t>
+  </si>
+  <si>
+    <t>take a couple deep breaths</t>
+  </si>
+  <si>
+    <t>we're going to get right back into it all right so we got ten seconds</t>
+  </si>
+  <si>
+    <t>i'm going to grab my dumbbells</t>
+  </si>
+  <si>
+    <t>we're getting ready</t>
+  </si>
+  <si>
+    <t>we're starting with the row</t>
+  </si>
+  <si>
+    <t>we're gonna doing my &lt;unk&gt; row &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>doing her t row and here we go</t>
+  </si>
+  <si>
+    <t>we're pulling back at those elbows keeping our core nice and tight and if you're wondering why we didn't take a longer break even though we're beginners that's because the workout specifically designed to allow some muscles to rest while others are working so right now our backs working but at the same time our chest may be resting allows us to get a lot done in a short period of time again pulling back on those elbows anytime</t>
+  </si>
+  <si>
+    <t>you're doing a row you want to be like you have a string attached to your elbows and you're just pulling back on it</t>
+  </si>
+  <si>
+    <t>just be sure to keep that core tight also exactly</t>
+  </si>
+  <si>
+    <t>you don't want your back getting loose or allowing your abs to relax almost there on this one</t>
+  </si>
+  <si>
+    <t>let's go five four three two and one all right going to the ground you need both weights for this next one doing that</t>
+  </si>
+  <si>
+    <t>hip up plus chest press</t>
+  </si>
+  <si>
+    <t>so we're driving off the heels and squeezing our &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>and pressing up at the same time nice work and again on any of these</t>
+  </si>
+  <si>
+    <t>don't feel like you have to use the same weight for all of them</t>
+  </si>
+  <si>
+    <t>feel free to adjust the way as you go through it</t>
+  </si>
+  <si>
+    <t>start with your best gas</t>
+  </si>
+  <si>
+    <t>but don't just keep the weight if it's not if you're not able to complete the reps in a safe manner or the other way if it's not challenging you make sure to up the weight so you can get that full benefit nice work driving off the heels pressing straight up keep it up guys almost there and five four three two one zero</t>
+  </si>
+  <si>
+    <t>we're up on our feet and try to keep the pace up a little bit faster for the second round</t>
+  </si>
+  <si>
+    <t>because we know what we're doing we're going to stiff leg &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>or our &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>shrug kick back</t>
+  </si>
+  <si>
+    <t>blow your knees hop in the truck taking the weight back on our hips feeling that stretch and up and shrug nice work</t>
+  </si>
+  <si>
+    <t>this one really hits that whole &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>chain so important i always say in your front are the show muscles in the back of the go muscles basically means all your power and real athleticism comes from your backside</t>
+  </si>
+  <si>
+    <t>come on keep it up you got it nice work not many left</t>
+  </si>
+  <si>
+    <t>let's go five more seconds</t>
+  </si>
+  <si>
+    <t>that's it and four three two one and zero finishing strong</t>
+  </si>
+  <si>
+    <t>okay grab your seat beam</t>
+  </si>
+  <si>
+    <t>got one so</t>
+  </si>
+  <si>
+    <t>if you're doing your shoulder press say get seated feel free to grab it otherwise kicking them up getting right into it bring those dumbbells down to about in line with your ears</t>
+  </si>
+  <si>
+    <t>maybe just a little bit lower really depends on your flexibility and what feels comfortable</t>
+  </si>
+  <si>
+    <t>don't take it to a place</t>
+  </si>
+  <si>
+    <t>it feels awkward with shoulders</t>
+  </si>
+  <si>
+    <t>nice work core stays tight</t>
+  </si>
+  <si>
+    <t>doesn't matter either one whichever one you're doing still stays tight nice work</t>
+  </si>
+  <si>
+    <t>this is about that point in the workout</t>
+  </si>
+  <si>
+    <t>where you start to really feel it it starts to kick in and it becomes all mental right now not even physical</t>
+  </si>
+  <si>
+    <t>it's all up in your head</t>
+  </si>
+  <si>
+    <t>it's all that mental &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>and grip that's going to keep you moving fighting</t>
+  </si>
+  <si>
+    <t>through rep by rep</t>
+  </si>
+  <si>
+    <t>let's go come on and five four three two one zero</t>
+  </si>
+  <si>
+    <t>ahh all right feeling good moving on to a dumbbell curls</t>
+  </si>
+  <si>
+    <t>we're hitting the biceps next</t>
+  </si>
+  <si>
+    <t>let's get it both curling at the same time curling those &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>in there we go arms are starting to be a little bit get a little bit lactic</t>
+  </si>
+  <si>
+    <t>acid built up in them</t>
+  </si>
+  <si>
+    <t>remember you don't have to listen to that</t>
+  </si>
+  <si>
+    <t>that's just a pain signal but the muscles got plenty left</t>
+  </si>
+  <si>
+    <t>you got this come on driving through curl those &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>in shoulders are back</t>
+  </si>
+  <si>
+    <t>nice work one</t>
+  </si>
+  <si>
+    <t>right into the next (2 second silence) good form not swinging the weights</t>
+  </si>
+  <si>
+    <t>not getting a bunch of momentum involved almost there go five more seconds</t>
+  </si>
+  <si>
+    <t>that's it and four three two one zero all right all right</t>
+  </si>
+  <si>
+    <t>we're moving on to either a dumbbell squat or a dumbbell goblet squat from the chair</t>
+  </si>
+  <si>
+    <t>i'll clean that name up later</t>
+  </si>
+  <si>
+    <t>okay so we're doing going into our squats weights back in our hips making sure to break at the hips every time</t>
+  </si>
+  <si>
+    <t>because if you don't what happens is you bend at the knees first and you end up here</t>
+  </si>
+  <si>
+    <t>and then you're like oh man</t>
+  </si>
+  <si>
+    <t>my knees hurt hips back then squat</t>
+  </si>
+  <si>
+    <t>that's the key</t>
+  </si>
+  <si>
+    <t>keep those feet flat drive off the heels nice work</t>
+  </si>
+  <si>
+    <t>you got it every squat you do</t>
+  </si>
+  <si>
+    <t>you're going to get that much better at it</t>
+  </si>
+  <si>
+    <t>nobody starts great at these</t>
+  </si>
+  <si>
+    <t>i promise you it's work putting in the work right here and you will see the results</t>
+  </si>
+  <si>
+    <t>i promise you come back repeat it better</t>
+  </si>
+  <si>
+    <t>that's what it's all about</t>
+  </si>
+  <si>
+    <t>thank you so much for your hard work today</t>
+  </si>
+  <si>
+    <t>nice work good we got it</t>
+  </si>
+  <si>
+    <t>let's go five four three two one and done okay</t>
+  </si>
+  <si>
+    <t>we're going back to the upper body &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>said while one body parts resting the others working so now we're going to the upper body dumbbell &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>kickbacks elbows are up only bennett those elbows extend and squeeze that back of the arm</t>
+  </si>
+  <si>
+    <t>squeeze those triceps</t>
+  </si>
+  <si>
+    <t>nice work guys come on keep it up one into the next this</t>
+  </si>
+  <si>
+    <t>is it right here</t>
+  </si>
+  <si>
+    <t>we don't have much left</t>
+  </si>
+  <si>
+    <t>we got</t>
+  </si>
+  <si>
+    <t>what about up one more exercise</t>
+  </si>
+  <si>
+    <t>i'll add one more after this one guys</t>
+  </si>
+  <si>
+    <t>that's it fighting through</t>
+  </si>
+  <si>
+    <t>it's all mental</t>
+  </si>
+  <si>
+    <t>remember focus on your goals focus on what brought you here</t>
+  </si>
+  <si>
+    <t>what motivates you and get there</t>
+  </si>
+  <si>
+    <t>breathe let's go and five four three two one and done okay</t>
+  </si>
+  <si>
+    <t>we're going to finish up with some abs</t>
+  </si>
+  <si>
+    <t>it means we're going to the ground</t>
+  </si>
+  <si>
+    <t>i'm gonna keep one body's gonna keep one this time two hands on once you'll go and we're going to go right into those reach crunches reaching up to the ceiling squeeze in those abs up at the top you got it</t>
+  </si>
+  <si>
+    <t>breathe remember this</t>
+  </si>
+  <si>
+    <t>what are you saving it for</t>
+  </si>
+  <si>
+    <t>don't save anything</t>
+  </si>
+  <si>
+    <t>put it all out there right now</t>
+  </si>
+  <si>
+    <t>right here right now</t>
+  </si>
+  <si>
+    <t>let's go nice work</t>
+  </si>
+  <si>
+    <t>nice work not much left more than halfway done with this one already here</t>
+  </si>
+  <si>
+    <t>we go rep by rep getting closer to the end</t>
+  </si>
+  <si>
+    <t>go through that finish line</t>
+  </si>
+  <si>
+    <t>almost there come on now in five four three two one zero nice work we are done</t>
+  </si>
+  <si>
+    <t>ah ah burn so good</t>
+  </si>
+  <si>
+    <t>thank you so much nice work girl</t>
+  </si>
+  <si>
+    <t>good job thank you so much for working out with us today</t>
+  </si>
+  <si>
+    <t>we couldn't do it without you literally</t>
+  </si>
+  <si>
+    <t>if you like this workout as much as we did make sure you give it a big &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>thumbs up and subscribe to this &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>channel it really helps us keep this great service free</t>
+  </si>
+  <si>
+    <t>make sure you check out has fit &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>where we have free workouts free meal plans and our complete fitness programs</t>
+  </si>
+  <si>
+    <t>don't forget to follow us on social media you can like us on &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>for in the know when our workouts come out say of the day subscribe go</t>
+  </si>
+  <si>
+    <t>show you some motivation</t>
+  </si>
+  <si>
+    <t>yeah i'd love to have you as a friend right</t>
+  </si>
+  <si>
+    <t>thank you so much for giving us the opportunity to serve you today</t>
+  </si>
+  <si>
+    <t>i'm coach &lt;unk&gt;</t>
+  </si>
+  <si>
+    <t>i'm claudia and we will see you at your next</t>
   </si>
 </sst>
 </file>
@@ -588,7 +1119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -613,7 +1144,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -632,10 +1163,10 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>57.00954794883728</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -643,10 +1174,10 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>98.27585816383362</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -668,7 +1199,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>74.29695129394531</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -676,10 +1207,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>99.99991655349731</v>
+        <v>71.73812985420227</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -687,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>99.99948740005493</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -701,7 +1232,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>99.99998807907104</v>
+        <v>77.35967636108398</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -709,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>99.99984502792358</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -745,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>99.99986886978149</v>
+        <v>68.17975640296936</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -756,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -767,7 +1298,7 @@
         <v>2</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>99.99892711639404</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -778,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>99.99960660934448</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -789,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>83.56537222862244</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -811,7 +1342,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>99.99998807907104</v>
+        <v>99.99978542327881</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -822,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -833,7 +1364,7 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <v>99.90358352661133</v>
+        <v>99.93937015533447</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -844,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>98.4968900680542</v>
+        <v>98.90754222869873</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -855,7 +1386,7 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>99.9998927116394</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -877,7 +1408,7 @@
         <v>2</v>
       </c>
       <c r="D26">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -888,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="D27">
-        <v>99.99982118606567</v>
+        <v>99.99980926513672</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -899,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <v>99.99998807907104</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -910,7 +1441,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>99.99780654907227</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -921,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>99.99996423721313</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -954,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <v>99.99922513961792</v>
+        <v>98.37700128555298</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -965,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="D34">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1009,7 +1540,7 @@
         <v>2</v>
       </c>
       <c r="D38">
-        <v>100</v>
+        <v>99.99927282333374</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1020,7 +1551,7 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>99.99984502792358</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1028,10 +1559,10 @@
         <v>41</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>99.99992847442627</v>
+        <v>99.96989965438843</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1042,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="D41">
-        <v>100</v>
+        <v>99.9983549118042</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1050,10 +1581,10 @@
         <v>43</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>63.54318857192993</v>
+        <v>95.96593379974365</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1064,7 +1595,7 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <v>57.46128559112549</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1075,7 +1606,7 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>99.99972581863403</v>
+        <v>99.99990463256836</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1086,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="D45">
-        <v>100</v>
+        <v>99.99974966049194</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1097,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <v>99.99939203262329</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1119,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <v>100</v>
+        <v>99.99839067459106</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1130,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="D49">
-        <v>99.99995231628418</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1141,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="D50">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1152,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="D51">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1163,7 +1694,7 @@
         <v>2</v>
       </c>
       <c r="D52">
-        <v>99.99994039535522</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1174,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="D53">
-        <v>99.99994039535522</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1196,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="D55">
-        <v>100</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1207,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="D56">
-        <v>81.78502321243286</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1218,7 +1749,7 @@
         <v>2</v>
       </c>
       <c r="D57">
-        <v>99.99979734420776</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1229,7 +1760,7 @@
         <v>2</v>
       </c>
       <c r="D58">
-        <v>99.99992847442627</v>
+        <v>99.9958872795105</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1240,7 +1771,7 @@
         <v>2</v>
       </c>
       <c r="D59">
-        <v>99.99655485153198</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1251,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <v>100</v>
+        <v>99.99415874481201</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1259,10 +1790,10 @@
         <v>62</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>99.99412298202515</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1273,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <v>99.99852180480957</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1284,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <v>100</v>
+        <v>99.99822378158569</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1303,10 +1834,10 @@
         <v>66</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <v>99.95394945144653</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1314,10 +1845,10 @@
         <v>67</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66">
-        <v>99.60540533065796</v>
+        <v>99.17632341384888</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1328,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <v>99.99817609786987</v>
+        <v>99.89436268806458</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1336,10 +1867,10 @@
         <v>69</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>100</v>
+        <v>98.61603975296021</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1350,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>99.87700581550598</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1361,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="D70">
-        <v>100</v>
+        <v>99.99995231628418</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1372,7 +1903,7 @@
         <v>2</v>
       </c>
       <c r="D71">
-        <v>99.99998807907104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1394,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="D73">
-        <v>99.99943971633911</v>
+        <v>99.99998807907104</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1405,7 +1936,7 @@
         <v>2</v>
       </c>
       <c r="D74">
-        <v>99.99985694885254</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1416,7 +1947,7 @@
         <v>2</v>
       </c>
       <c r="D75">
-        <v>100</v>
+        <v>99.8740017414093</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1427,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>91.51563048362732</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1438,7 +1969,7 @@
         <v>2</v>
       </c>
       <c r="D77">
-        <v>100</v>
+        <v>99.99996423721313</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1446,10 +1977,10 @@
         <v>79</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78">
-        <v>99.99386072158813</v>
+        <v>99.99997615814209</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1457,10 +1988,1968 @@
         <v>80</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79">
         <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>98.70562553405762</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>99.94288086891174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C84">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>99.99969005584717</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>99.99954700469971</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>99.73219037055969</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>99.99996423721313</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>99.99666213989258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>99.99053478240967</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>99.83615279197693</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>99.9707043170929</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>78.83683443069458</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <v>99.99969005584717</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>102</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>99.74662065505981</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>103</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>99.64814186096191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>104</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>99.99934434890747</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>99.99979734420776</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>99.90315437316895</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <v>99.99802112579346</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114">
+        <v>99.9990701675415</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>117</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <v>99.99964237213135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>118</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>119</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>99.99990463256836</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120">
+        <v>99.99991655349731</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>123</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <v>99.99982118606567</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>124</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>125</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+      <c r="D124">
+        <v>99.99969005584717</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>128</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>99.99991655349731</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>129</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>130</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>131</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130">
+        <v>95.62875628471375</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>133</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <v>99.99953508377075</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>134</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>135</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+      <c r="D134">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>136</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>137</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>99.6631920337677</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>138</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137">
+        <v>99.99932050704956</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>140</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>95.8920419216156</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>141</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>142</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>99.99978542327881</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>143</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+      <c r="D142">
+        <v>90.11827111244202</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>144</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>99.99970197677612</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>145</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144">
+        <v>99.86878037452698</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>146</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>99.99719858169556</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>147</v>
+      </c>
+      <c r="C146">
+        <v>2</v>
+      </c>
+      <c r="D146">
+        <v>98.48223924636841</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>148</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+      <c r="D147">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>149</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>150</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>151</v>
+      </c>
+      <c r="C150">
+        <v>2</v>
+      </c>
+      <c r="D150">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>152</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+      <c r="D151">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>153</v>
+      </c>
+      <c r="C152">
+        <v>2</v>
+      </c>
+      <c r="D152">
+        <v>99.99935626983643</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>154</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <v>99.99933242797852</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
+      <c r="D154">
+        <v>99.9997615814209</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>156</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155">
+        <v>99.99995231628418</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>157</v>
+      </c>
+      <c r="C156">
+        <v>2</v>
+      </c>
+      <c r="D156">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>158</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+      <c r="D157">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>159</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+      <c r="D158">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>160</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+      <c r="D159">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>161</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>99.9839186668396</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>162</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+      <c r="D161">
+        <v>99.9998927116394</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>163</v>
+      </c>
+      <c r="C162">
+        <v>2</v>
+      </c>
+      <c r="D162">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>164</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>165</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>166</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>167</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+      <c r="D166">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>168</v>
+      </c>
+      <c r="C167">
+        <v>2</v>
+      </c>
+      <c r="D167">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>169</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>170</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>171</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>172</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>99.99911785125732</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>173</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>60.23491024971008</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>174</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173">
+        <v>99.99996423721313</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>175</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+      <c r="D174">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>176</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>177</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>99.98717308044434</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>178</v>
+      </c>
+      <c r="C177">
+        <v>2</v>
+      </c>
+      <c r="D177">
+        <v>99.61115717887878</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>179</v>
+      </c>
+      <c r="C178">
+        <v>2</v>
+      </c>
+      <c r="D178">
+        <v>99.99986886978149</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>180</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+      <c r="D179">
+        <v>99.99978542327881</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>181</v>
+      </c>
+      <c r="C180">
+        <v>2</v>
+      </c>
+      <c r="D180">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>182</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>98.11734557151794</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>183</v>
+      </c>
+      <c r="C182">
+        <v>2</v>
+      </c>
+      <c r="D182">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>184</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183">
+        <v>99.94761347770691</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>185</v>
+      </c>
+      <c r="C184">
+        <v>2</v>
+      </c>
+      <c r="D184">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>186</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+      <c r="D185">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>187</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+      <c r="D186">
+        <v>99.96678829193115</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>188</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>189</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188">
+        <v>99.68830943107605</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>190</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+      <c r="D189">
+        <v>99.99996423721313</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="s">
+        <v>191</v>
+      </c>
+      <c r="C190">
+        <v>2</v>
+      </c>
+      <c r="D190">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" t="s">
+        <v>192</v>
+      </c>
+      <c r="C191">
+        <v>2</v>
+      </c>
+      <c r="D191">
+        <v>99.99985694885254</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="s">
+        <v>193</v>
+      </c>
+      <c r="C192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>99.97499585151672</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193">
+        <v>2</v>
+      </c>
+      <c r="D193">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194">
+        <v>2</v>
+      </c>
+      <c r="D194">
+        <v>99.99961853027344</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="s">
+        <v>196</v>
+      </c>
+      <c r="C195">
+        <v>2</v>
+      </c>
+      <c r="D195">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>197</v>
+      </c>
+      <c r="C196">
+        <v>2</v>
+      </c>
+      <c r="D196">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>198</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>199</v>
+      </c>
+      <c r="C198">
+        <v>2</v>
+      </c>
+      <c r="D198">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="s">
+        <v>200</v>
+      </c>
+      <c r="C199">
+        <v>2</v>
+      </c>
+      <c r="D199">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>201</v>
+      </c>
+      <c r="C200">
+        <v>2</v>
+      </c>
+      <c r="D200">
+        <v>99.97935891151428</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="s">
+        <v>202</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+      <c r="D201">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="s">
+        <v>203</v>
+      </c>
+      <c r="C202">
+        <v>2</v>
+      </c>
+      <c r="D202">
+        <v>99.99251365661621</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" t="s">
+        <v>204</v>
+      </c>
+      <c r="C203">
+        <v>2</v>
+      </c>
+      <c r="D203">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" t="s">
+        <v>205</v>
+      </c>
+      <c r="C204">
+        <v>2</v>
+      </c>
+      <c r="D204">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="s">
+        <v>206</v>
+      </c>
+      <c r="C205">
+        <v>2</v>
+      </c>
+      <c r="D205">
+        <v>99.99985694885254</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
+        <v>207</v>
+      </c>
+      <c r="C206">
+        <v>2</v>
+      </c>
+      <c r="D206">
+        <v>99.97120499610901</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>208</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" t="s">
+        <v>209</v>
+      </c>
+      <c r="C208">
+        <v>2</v>
+      </c>
+      <c r="D208">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" t="s">
+        <v>210</v>
+      </c>
+      <c r="C209">
+        <v>2</v>
+      </c>
+      <c r="D209">
+        <v>99.99983310699463</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" t="s">
+        <v>211</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" t="s">
+        <v>212</v>
+      </c>
+      <c r="C211">
+        <v>2</v>
+      </c>
+      <c r="D211">
+        <v>99.950110912323</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" t="s">
+        <v>213</v>
+      </c>
+      <c r="C212">
+        <v>2</v>
+      </c>
+      <c r="D212">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" t="s">
+        <v>214</v>
+      </c>
+      <c r="C213">
+        <v>2</v>
+      </c>
+      <c r="D213">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" t="s">
+        <v>215</v>
+      </c>
+      <c r="C214">
+        <v>2</v>
+      </c>
+      <c r="D214">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" t="s">
+        <v>216</v>
+      </c>
+      <c r="C215">
+        <v>2</v>
+      </c>
+      <c r="D215">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" t="s">
+        <v>217</v>
+      </c>
+      <c r="C216">
+        <v>2</v>
+      </c>
+      <c r="D216">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" t="s">
+        <v>218</v>
+      </c>
+      <c r="C217">
+        <v>2</v>
+      </c>
+      <c r="D217">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" t="s">
+        <v>219</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>99.9944806098938</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219" t="s">
+        <v>220</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219">
+        <v>99.99933242797852</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" t="s">
+        <v>221</v>
+      </c>
+      <c r="C220">
+        <v>2</v>
+      </c>
+      <c r="D220">
+        <v>99.99982118606567</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" t="s">
+        <v>222</v>
+      </c>
+      <c r="C221">
+        <v>2</v>
+      </c>
+      <c r="D221">
+        <v>99.99988079071045</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" t="s">
+        <v>223</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222">
+        <v>84.56353545188904</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" t="s">
+        <v>224</v>
+      </c>
+      <c r="C223">
+        <v>2</v>
+      </c>
+      <c r="D223">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" t="s">
+        <v>225</v>
+      </c>
+      <c r="C224">
+        <v>2</v>
+      </c>
+      <c r="D224">
+        <v>99.97135996818542</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" t="s">
+        <v>226</v>
+      </c>
+      <c r="C225">
+        <v>2</v>
+      </c>
+      <c r="D225">
+        <v>99.99741315841675</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226" t="s">
+        <v>227</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>99.99692440032959</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="s">
+        <v>228</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
+      <c r="D227">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228" t="s">
+        <v>229</v>
+      </c>
+      <c r="C228">
+        <v>2</v>
+      </c>
+      <c r="D228">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229" t="s">
+        <v>230</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+      <c r="D229">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230" t="s">
+        <v>231</v>
+      </c>
+      <c r="C230">
+        <v>2</v>
+      </c>
+      <c r="D230">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231" t="s">
+        <v>232</v>
+      </c>
+      <c r="C231">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232" t="s">
+        <v>219</v>
+      </c>
+      <c r="C232">
+        <v>2</v>
+      </c>
+      <c r="D232">
+        <v>99.9944806098938</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233" t="s">
+        <v>233</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <v>99.98773336410522</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234" t="s">
+        <v>234</v>
+      </c>
+      <c r="C234">
+        <v>2</v>
+      </c>
+      <c r="D234">
+        <v>74.86447691917419</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235" t="s">
+        <v>235</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>99.99996423721313</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236" t="s">
+        <v>236</v>
+      </c>
+      <c r="C236">
+        <v>2</v>
+      </c>
+      <c r="D236">
+        <v>62.27043867111206</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237" t="s">
+        <v>237</v>
+      </c>
+      <c r="C237">
+        <v>2</v>
+      </c>
+      <c r="D237">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238" t="s">
+        <v>238</v>
+      </c>
+      <c r="C238">
+        <v>2</v>
+      </c>
+      <c r="D238">
+        <v>99.43974018096924</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" t="s">
+        <v>239</v>
+      </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
+      <c r="D239">
+        <v>99.9919056892395</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" t="s">
+        <v>240</v>
+      </c>
+      <c r="C240">
+        <v>2</v>
+      </c>
+      <c r="D240">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" t="s">
+        <v>241</v>
+      </c>
+      <c r="C241">
+        <v>2</v>
+      </c>
+      <c r="D241">
+        <v>99.99998807907104</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242" t="s">
+        <v>242</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242">
+        <v>99.99994039535522</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" t="s">
+        <v>243</v>
+      </c>
+      <c r="C243">
+        <v>1</v>
+      </c>
+      <c r="D243">
+        <v>99.99995231628418</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" t="s">
+        <v>244</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" t="s">
+        <v>245</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" t="s">
+        <v>246</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246">
+        <v>99.99997615814209</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247" t="s">
+        <v>247</v>
+      </c>
+      <c r="C247">
+        <v>2</v>
+      </c>
+      <c r="D247">
+        <v>87.09980249404907</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248" t="s">
+        <v>248</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249" t="s">
+        <v>249</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250" t="s">
+        <v>250</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251" t="s">
+        <v>251</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251">
+        <v>99.99996423721313</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" t="s">
+        <v>252</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" t="s">
+        <v>253</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
+      <c r="D253">
+        <v>99.99994039535522</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" t="s">
+        <v>254</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255" t="s">
+        <v>255</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256" t="s">
+        <v>256</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257" t="s">
+        <v>257</v>
+      </c>
+      <c r="C257">
+        <v>1</v>
+      </c>
+      <c r="D257">
+        <v>99.99998807907104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>